<commit_message>
Update Bill of Materials-shepherd_target_nRF.xlsx
</commit_message>
<xml_diff>
--- a/PCBs/target_nRF52_v2.1r0/Bill of Materials-shepherd_target_nRF.xlsx
+++ b/PCBs/target_nRF52_v2.1r0/Bill of Materials-shepherd_target_nRF.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\Projects\shepherd_v2_nRF_Target\Project Outputs for shepherd_v2_nRF_Target\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ingmo\Documents\GitHub\shepherd_v2_planning\PCBs\target_nRF52_v2.1r0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5505E45-7656-49F8-BCD9-BC2727554EC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9DDDD3-3AF1-4096-B265-6822BB8BE493}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6384" yWindow="2376" windowWidth="23016" windowHeight="14376" xr2:uid="{AEC7E32C-3D66-4E83-BB24-487AB1644DA6}"/>
+    <workbookView xWindow="768" yWindow="7596" windowWidth="36360" windowHeight="17976" xr2:uid="{AEC7E32C-3D66-4E83-BB24-487AB1644DA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-shepherd_targ" sheetId="1" r:id="rId1"/>
@@ -709,9 +709,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -719,7 +721,7 @@
     <col min="7" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -753,8 +755,11 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -788,8 +793,15 @@
       <c r="K2" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="L2">
+        <f>F2*L$1</f>
+        <v>96</v>
+      </c>
+      <c r="M2">
+        <v>800</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
@@ -823,8 +835,15 @@
       <c r="K3" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L13" si="0">F3*L$1</f>
+        <v>64</v>
+      </c>
+      <c r="M3">
+        <v>74</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
@@ -858,8 +877,15 @@
       <c r="K4" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="M4">
+        <v>30</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>39</v>
       </c>
@@ -893,8 +919,15 @@
       <c r="K5" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="M5">
+        <v>32</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>48</v>
       </c>
@@ -928,8 +961,15 @@
       <c r="K6" s="3" t="s">
         <v>56</v>
       </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="M6">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>57</v>
       </c>
@@ -955,8 +995,15 @@
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>61</v>
       </c>
@@ -990,8 +1037,15 @@
       <c r="K8" s="3" t="s">
         <v>69</v>
       </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="M8">
+        <v>1050</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>70</v>
       </c>
@@ -1025,8 +1079,18 @@
       <c r="K9" s="3" t="s">
         <v>69</v>
       </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="M9">
+        <v>10</v>
+      </c>
+      <c r="N9">
+        <v>100</v>
+      </c>
     </row>
-    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>75</v>
       </c>
@@ -1060,8 +1124,15 @@
       <c r="K10" s="3" t="s">
         <v>69</v>
       </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="M10">
+        <v>128</v>
+      </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>80</v>
       </c>
@@ -1087,8 +1158,12 @@
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>84</v>
       </c>
@@ -1122,8 +1197,15 @@
       <c r="K12" s="3" t="s">
         <v>91</v>
       </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="M12">
+        <v>64</v>
+      </c>
     </row>
-    <row r="13" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>92</v>
       </c>
@@ -1156,6 +1238,16 @@
       </c>
       <c r="K13" s="3" t="s">
         <v>97</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="M13">
+        <v>29</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>